<commit_message>
Added number of criteria for metabolic syndrome (MS_5cri))
</commit_message>
<xml_diff>
--- a/Assignment 1/KIM_codebook.xlsx
+++ b/Assignment 1/KIM_codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UCLA_PhD_Epi\2022_1Winter\EPIDEM207_Reproducibility_in_epidemiology_research\EPIDEM207_Git\EPIDEM207-2022\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5018847-7424-4780-96B5-3185C1DDF07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D6AF45-3B75-42A8-B4FB-D6FDE0FE602E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B419D853-1A87-483E-B32B-D807339D7DF2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
   <si>
     <t>Number</t>
   </si>
@@ -225,18 +225,6 @@
     <t>Missing percent</t>
   </si>
   <si>
-    <t>1st quartile</t>
-  </si>
-  <si>
-    <t>2nd quartile</t>
-  </si>
-  <si>
-    <t>3rd quartile</t>
-  </si>
-  <si>
-    <t>4th quartile</t>
-  </si>
-  <si>
     <t>Min</t>
   </si>
   <si>
@@ -301,6 +289,24 @@
   </si>
   <si>
     <t>C-reactive protein (mg/L)</t>
+  </si>
+  <si>
+    <t>MS_5cri</t>
+  </si>
+  <si>
+    <t>Metabolic syndrome, number of criteria</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
   </si>
 </sst>
 </file>
@@ -342,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -351,6 +357,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F7C037-C9E8-4565-8747-61942B8DB76A}">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,10 +709,10 @@
         <v>48</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>49</v>
@@ -822,7 +831,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -851,7 +860,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -880,7 +889,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -909,7 +918,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -938,7 +947,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -967,7 +976,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -996,7 +1005,7 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -1062,16 +1071,22 @@
       <c r="K14">
         <v>16.43</v>
       </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -1079,149 +1094,110 @@
       <c r="H15" s="2">
         <v>0</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>54</v>
+      <c r="I15" s="4">
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>9390</v>
+        <v>4891</v>
       </c>
       <c r="K15">
-        <v>68.94</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="3">
-        <v>0</v>
+        <v>35.909999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H16" s="2">
         <v>1</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>55</v>
+      <c r="I16" s="4">
+        <v>1</v>
       </c>
       <c r="J16">
-        <v>4230</v>
+        <v>3797</v>
       </c>
       <c r="K16">
-        <v>31.06</v>
+        <v>27.88</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
       <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>54</v>
+        <v>2</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2</v>
       </c>
       <c r="J17">
-        <v>12481</v>
+        <v>2694</v>
       </c>
       <c r="K17">
-        <v>91.64</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="3">
-        <v>0</v>
+        <v>19.78</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H18" s="2">
-        <v>1</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>55</v>
+        <v>3</v>
+      </c>
+      <c r="I18" s="4">
+        <v>3</v>
       </c>
       <c r="J18">
-        <v>1139</v>
+        <v>1513</v>
       </c>
       <c r="K18">
-        <v>8.36</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
       <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>54</v>
+        <v>4</v>
+      </c>
+      <c r="I19" s="4">
+        <v>4</v>
       </c>
       <c r="J19">
-        <v>8549</v>
+        <v>605</v>
       </c>
       <c r="K19">
-        <v>62.77</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="3">
-        <v>0</v>
+        <v>4.4400000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>55</v>
+        <v>5</v>
+      </c>
+      <c r="I20" s="4">
+        <v>5</v>
       </c>
       <c r="J20">
-        <v>5071</v>
+        <v>120</v>
       </c>
       <c r="K20">
-        <v>37.229999999999997</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="3">
-        <v>166.1874756</v>
-      </c>
-      <c r="F21" s="3">
-        <v>136.80000000000001</v>
-      </c>
-      <c r="G21" s="3">
-        <v>210</v>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J21">
+        <v>9390</v>
+      </c>
+      <c r="K21">
+        <v>68.94</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -1231,55 +1207,43 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="3">
-        <v>65.858604999999997</v>
-      </c>
-      <c r="F22" s="3">
-        <v>33.700000000000003</v>
-      </c>
-      <c r="G22" s="3">
-        <v>185.4</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22" s="3">
-        <v>0</v>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22">
+        <v>4230</v>
+      </c>
+      <c r="K22">
+        <v>31.06</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="3">
-        <v>83.567555100000007</v>
-      </c>
-      <c r="F23" s="3">
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="3">
-        <v>155</v>
+      <c r="J23">
+        <v>12481</v>
+      </c>
+      <c r="K23">
+        <v>91.64</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -1289,43 +1253,28 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>18</v>
-      </c>
-      <c r="B24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="3">
-        <v>23.706800300000001</v>
-      </c>
-      <c r="F24" s="3">
-        <v>14.3</v>
-      </c>
-      <c r="G24" s="3">
-        <v>68.099999999999994</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24" s="3">
-        <v>0</v>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24">
+        <v>1139</v>
+      </c>
+      <c r="K24">
+        <v>8.36</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
@@ -1337,10 +1286,10 @@
         <v>54</v>
       </c>
       <c r="J25">
-        <v>9164</v>
+        <v>8549</v>
       </c>
       <c r="K25">
-        <v>67.28</v>
+        <v>62.77</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -1357,33 +1306,33 @@
         <v>55</v>
       </c>
       <c r="J26">
-        <v>4456</v>
+        <v>5071</v>
       </c>
       <c r="K26">
-        <v>32.72</v>
+        <v>37.229999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="3">
-        <v>117.473348</v>
+        <v>166.1874756</v>
       </c>
       <c r="F27" s="3">
-        <v>66</v>
+        <v>136.80000000000001</v>
       </c>
       <c r="G27" s="3">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -1394,25 +1343,25 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="3">
-        <v>79.099412599999994</v>
+        <v>65.858604999999997</v>
       </c>
       <c r="F28" s="3">
-        <v>41</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="G28" s="3">
-        <v>135</v>
+        <v>185.4</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -1423,25 +1372,25 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="3">
-        <v>19.808595</v>
+        <v>83.567555100000007</v>
       </c>
       <c r="F29" s="3">
-        <v>8.43</v>
+        <v>54</v>
       </c>
       <c r="G29" s="3">
-        <v>42.22</v>
+        <v>155</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -1452,25 +1401,25 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="3">
-        <v>29.9354741</v>
+        <v>23.706800300000001</v>
       </c>
       <c r="F30" s="3">
-        <v>16.546242800000002</v>
+        <v>14.3</v>
       </c>
       <c r="G30" s="3">
-        <v>49.743178200000003</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -1481,28 +1430,28 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J31">
-        <v>3405</v>
+        <v>9164</v>
       </c>
       <c r="K31">
-        <v>25</v>
+        <v>67.28</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -1513,70 +1462,97 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H32" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="J32">
-        <v>3405</v>
+        <v>4456</v>
       </c>
       <c r="K32">
-        <v>25</v>
+        <v>32.72</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H33" s="2">
-        <v>3</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J33">
-        <v>3405</v>
-      </c>
-      <c r="K33">
-        <v>25</v>
+      <c r="A33">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="3">
+        <v>117.473348</v>
+      </c>
+      <c r="F33" s="3">
+        <v>66</v>
+      </c>
+      <c r="G33" s="3">
+        <v>193</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H34" s="2">
-        <v>4</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J34">
-        <v>3405</v>
-      </c>
-      <c r="K34">
-        <v>25</v>
+      <c r="A34">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="3">
+        <v>79.099412599999994</v>
+      </c>
+      <c r="F34" s="3">
+        <v>41</v>
+      </c>
+      <c r="G34" s="3">
+        <v>135</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
       </c>
-      <c r="H35" s="2">
-        <v>0</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J35">
-        <v>12554</v>
-      </c>
-      <c r="K35">
-        <v>92.17</v>
+      <c r="E35" s="3">
+        <v>19.808595</v>
+      </c>
+      <c r="F35" s="3">
+        <v>8.43</v>
+      </c>
+      <c r="G35" s="3">
+        <v>42.22</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -1586,40 +1562,58 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H36" s="2">
-        <v>1</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J36">
-        <v>1066</v>
-      </c>
-      <c r="K36">
-        <v>7.83</v>
+      <c r="A36">
+        <v>24</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="3">
+        <v>29.9354741</v>
+      </c>
+      <c r="F36" s="3">
+        <v>16.546242800000002</v>
+      </c>
+      <c r="G36" s="3">
+        <v>49.743178200000003</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D37" t="s">
         <v>5</v>
       </c>
-      <c r="E37" s="3">
-        <v>91.485110500000005</v>
-      </c>
-      <c r="F37" s="3">
-        <v>5</v>
-      </c>
-      <c r="G37" s="3">
-        <v>400.9</v>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J37">
+        <v>3405</v>
+      </c>
+      <c r="K37">
+        <v>25</v>
       </c>
       <c r="L37">
         <v>0</v>
@@ -1629,147 +1623,114 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>27</v>
-      </c>
-      <c r="B38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" t="s">
-        <v>5</v>
-      </c>
       <c r="H38" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="J38">
-        <v>11239</v>
+        <v>3405</v>
       </c>
       <c r="K38">
-        <v>82.52</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38" s="3">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H39" s="2">
+        <v>3</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J39">
+        <v>3405</v>
+      </c>
+      <c r="K39">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H40" s="2">
+        <v>4</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J40">
+        <v>3405</v>
+      </c>
+      <c r="K40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>26</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J41">
+        <v>12554</v>
+      </c>
+      <c r="K41">
+        <v>92.17</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H42" s="2">
         <v>1</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J39">
-        <v>2381</v>
-      </c>
-      <c r="K39">
-        <v>17.48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>28</v>
-      </c>
-      <c r="B40" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" t="s">
-        <v>5</v>
-      </c>
-      <c r="H40" s="2">
-        <v>0</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J40">
-        <v>6396</v>
-      </c>
-      <c r="K40">
-        <v>46.96</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H41" s="2">
-        <v>1</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J41">
-        <v>7224</v>
-      </c>
-      <c r="K41">
-        <v>53.04</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>29</v>
-      </c>
-      <c r="B42" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="3">
-        <v>9.6511475000000004</v>
-      </c>
-      <c r="F42" s="3">
-        <v>1.7</v>
-      </c>
-      <c r="G42" s="3">
-        <v>48.9</v>
-      </c>
-      <c r="L42">
-        <v>13315</v>
-      </c>
-      <c r="M42" s="3">
-        <v>97.760646108663735</v>
+      <c r="J42">
+        <v>1066</v>
+      </c>
+      <c r="K42">
+        <v>7.83</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
         <v>5</v>
       </c>
       <c r="E43" s="3">
-        <v>5.6249419999999999</v>
+        <v>91.485110500000005</v>
       </c>
       <c r="F43" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G43" s="3">
-        <v>14.1</v>
+        <v>400.9</v>
       </c>
       <c r="L43">
         <v>0</v>
@@ -1780,71 +1741,59 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
       </c>
-      <c r="E44" s="3">
-        <v>5.2450988000000001</v>
-      </c>
-      <c r="F44" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="G44" s="3">
-        <v>13.4</v>
+      <c r="H44" s="2">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J44">
+        <v>11239</v>
+      </c>
+      <c r="K44">
+        <v>82.52</v>
       </c>
       <c r="L44">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="M44" s="3">
-        <v>1.5051395007342145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>32</v>
-      </c>
-      <c r="B45" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="3">
-        <v>0.1485852</v>
-      </c>
-      <c r="F45" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="G45" s="3">
-        <v>20.89</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45" s="3">
-        <v>0</v>
+      <c r="H45" s="2">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J45">
+        <v>2381</v>
+      </c>
+      <c r="K45">
+        <v>17.48</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
@@ -1853,13 +1802,13 @@
         <v>0</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J46">
-        <v>553</v>
+        <v>6396</v>
       </c>
       <c r="K46">
-        <v>4.0599999999999996</v>
+        <v>46.96</v>
       </c>
       <c r="L46">
         <v>0</v>
@@ -1872,41 +1821,203 @@
       <c r="H47" s="2">
         <v>1</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J47">
+        <v>7224</v>
+      </c>
+      <c r="K47">
+        <v>53.04</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>30</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="3">
+        <v>9.6511475000000004</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="G48" s="3">
+        <v>48.9</v>
+      </c>
+      <c r="L48">
+        <v>13315</v>
+      </c>
+      <c r="M48" s="3">
+        <v>97.760646108663735</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>31</v>
+      </c>
+      <c r="B49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="3">
+        <v>5.6249419999999999</v>
+      </c>
+      <c r="F49" s="3">
+        <v>3</v>
+      </c>
+      <c r="G49" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>32</v>
+      </c>
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="3">
+        <v>5.2450988000000001</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G50" s="3">
+        <v>13.4</v>
+      </c>
+      <c r="L50">
+        <v>205</v>
+      </c>
+      <c r="M50" s="3">
+        <v>1.5051395007342145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>33</v>
+      </c>
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.1485852</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="G51" s="3">
+        <v>20.89</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>34</v>
+      </c>
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" t="s">
+        <v>47</v>
+      </c>
+      <c r="D52" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J52">
+        <v>553</v>
+      </c>
+      <c r="K52">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H53" s="2">
+        <v>1</v>
+      </c>
+      <c r="I53" t="s">
         <v>57</v>
       </c>
-      <c r="J47">
+      <c r="J53">
         <v>5345</v>
       </c>
-      <c r="K47">
+      <c r="K53">
         <v>39.24</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H48" s="2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H54" s="2">
         <v>2</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I54" t="s">
         <v>58</v>
       </c>
-      <c r="J48">
+      <c r="J54">
         <v>3266</v>
       </c>
-      <c r="K48">
+      <c r="K54">
         <v>23.98</v>
       </c>
     </row>
-    <row r="49" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H49" s="2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H55" s="2">
         <v>3</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I55" t="s">
         <v>59</v>
       </c>
-      <c r="J49">
+      <c r="J55">
         <v>4456</v>
       </c>
-      <c r="K49">
+      <c r="K55">
         <v>32.72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated assignment 1 part C code
</commit_message>
<xml_diff>
--- a/Assignment 1/KIM_codebook.xlsx
+++ b/Assignment 1/KIM_codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UCLA_PhD_Epi\2022_1Winter\EPIDEM207_Reproducibility_in_epidemiology_research\EPIDEM207_Git\EPIDEM207-2022\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D6AF45-3B75-42A8-B4FB-D6FDE0FE602E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D7A1D0-1977-48F0-B07E-F995388DC91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B419D853-1A87-483E-B32B-D807339D7DF2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
   <si>
     <t>Number</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>Q4</t>
+  </si>
+  <si>
+    <t>VFA_</t>
+  </si>
+  <si>
+    <t>Visceral obesity</t>
   </si>
 </sst>
 </file>
@@ -674,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F7C037-C9E8-4565-8747-61942B8DB76A}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1744,10 +1750,10 @@
         <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
@@ -1757,18 +1763,6 @@
       </c>
       <c r="I44" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="J44">
-        <v>11239</v>
-      </c>
-      <c r="K44">
-        <v>82.52</v>
-      </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-      <c r="M44" s="3">
-        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
@@ -1778,22 +1772,16 @@
       <c r="I45" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J45">
-        <v>2381</v>
-      </c>
-      <c r="K45">
-        <v>17.48</v>
-      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
@@ -1805,10 +1793,10 @@
         <v>54</v>
       </c>
       <c r="J46">
-        <v>6396</v>
+        <v>11239</v>
       </c>
       <c r="K46">
-        <v>46.96</v>
+        <v>82.52</v>
       </c>
       <c r="L46">
         <v>0</v>
@@ -1825,120 +1813,108 @@
         <v>55</v>
       </c>
       <c r="J47">
-        <v>7224</v>
+        <v>2381</v>
       </c>
       <c r="K47">
-        <v>53.04</v>
+        <v>17.48</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D48" t="s">
         <v>5</v>
       </c>
-      <c r="E48" s="3">
-        <v>9.6511475000000004</v>
-      </c>
-      <c r="F48" s="3">
-        <v>1.7</v>
-      </c>
-      <c r="G48" s="3">
-        <v>48.9</v>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J48">
+        <v>6396</v>
+      </c>
+      <c r="K48">
+        <v>46.96</v>
       </c>
       <c r="L48">
-        <v>13315</v>
+        <v>0</v>
       </c>
       <c r="M48" s="3">
-        <v>97.760646108663735</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>31</v>
-      </c>
-      <c r="B49" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" t="s">
-        <v>82</v>
-      </c>
-      <c r="D49" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="3">
-        <v>5.6249419999999999</v>
-      </c>
-      <c r="F49" s="3">
-        <v>3</v>
-      </c>
-      <c r="G49" s="3">
-        <v>14.1</v>
-      </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49" s="3">
-        <v>0</v>
+      <c r="H49" s="2">
+        <v>1</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J49">
+        <v>7224</v>
+      </c>
+      <c r="K49">
+        <v>53.04</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C50" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="D50" t="s">
         <v>5</v>
       </c>
       <c r="E50" s="3">
-        <v>5.2450988000000001</v>
+        <v>9.6511475000000004</v>
       </c>
       <c r="F50" s="3">
-        <v>0.1</v>
+        <v>1.7</v>
       </c>
       <c r="G50" s="3">
-        <v>13.4</v>
+        <v>48.9</v>
       </c>
       <c r="L50">
-        <v>205</v>
+        <v>13315</v>
       </c>
       <c r="M50" s="3">
-        <v>1.5051395007342145</v>
+        <v>97.760646108663735</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D51" t="s">
         <v>5</v>
       </c>
       <c r="E51" s="3">
-        <v>0.1485852</v>
+        <v>5.6249419999999999</v>
       </c>
       <c r="F51" s="3">
-        <v>0.02</v>
+        <v>3</v>
       </c>
       <c r="G51" s="3">
-        <v>20.89</v>
+        <v>14.1</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -1949,75 +1925,133 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52">
+        <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="3">
+        <v>5.2450988000000001</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G52" s="3">
+        <v>13.4</v>
+      </c>
+      <c r="L52">
+        <v>205</v>
+      </c>
+      <c r="M52" s="3">
+        <v>1.5051395007342145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>33</v>
+      </c>
+      <c r="B53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0.1485852</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="G53" s="3">
+        <v>20.89</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A54">
         <v>34</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>46</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>47</v>
       </c>
-      <c r="D52" t="s">
-        <v>5</v>
-      </c>
-      <c r="H52" s="2">
-        <v>0</v>
-      </c>
-      <c r="I52" s="1" t="s">
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J52">
+      <c r="J54">
         <v>553</v>
       </c>
-      <c r="K52">
+      <c r="K54">
         <v>4.0599999999999996</v>
       </c>
-      <c r="L52">
-        <v>0</v>
-      </c>
-      <c r="M52" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H53" s="2">
-        <v>1</v>
-      </c>
-      <c r="I53" t="s">
-        <v>57</v>
-      </c>
-      <c r="J53">
-        <v>5345</v>
-      </c>
-      <c r="K53">
-        <v>39.24</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H54" s="2">
-        <v>2</v>
-      </c>
-      <c r="I54" t="s">
-        <v>58</v>
-      </c>
-      <c r="J54">
-        <v>3266</v>
-      </c>
-      <c r="K54">
-        <v>23.98</v>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H55" s="2">
+        <v>1</v>
+      </c>
+      <c r="I55" t="s">
+        <v>57</v>
+      </c>
+      <c r="J55">
+        <v>5345</v>
+      </c>
+      <c r="K55">
+        <v>39.24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H56" s="2">
+        <v>2</v>
+      </c>
+      <c r="I56" t="s">
+        <v>58</v>
+      </c>
+      <c r="J56">
+        <v>3266</v>
+      </c>
+      <c r="K56">
+        <v>23.98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H57" s="2">
         <v>3</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I57" t="s">
         <v>59</v>
       </c>
-      <c r="J55">
+      <c r="J57">
         <v>4456</v>
       </c>
-      <c r="K55">
+      <c r="K57">
         <v>32.72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated codebook and data dictionary
</commit_message>
<xml_diff>
--- a/Assignment 1/KIM_codebook.xlsx
+++ b/Assignment 1/KIM_codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UCLA_PhD_Epi\2022_1Winter\EPIDEM207_Reproducibility_in_epidemiology_research\EPIDEM207_Git\EPIDEM207-2022\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D7A1D0-1977-48F0-B07E-F995388DC91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397FF3FF-1B2D-47AB-B29E-BAD7929A634D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B419D853-1A87-483E-B32B-D807339D7DF2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
   <si>
     <t>Number</t>
   </si>
@@ -313,6 +313,39 @@
   </si>
   <si>
     <t>Visceral obesity</t>
+  </si>
+  <si>
+    <t>Underweight</t>
+  </si>
+  <si>
+    <t>Underweight (BMI &lt;18.5 kg/m^2)</t>
+  </si>
+  <si>
+    <t>Character</t>
+  </si>
+  <si>
+    <t>Agegroup</t>
+  </si>
+  <si>
+    <t>Age group (years)</t>
+  </si>
+  <si>
+    <t>20-29 years</t>
+  </si>
+  <si>
+    <t>30-39 years</t>
+  </si>
+  <si>
+    <t>40-49 years</t>
+  </si>
+  <si>
+    <t>50-59 years</t>
+  </si>
+  <si>
+    <t>60-69 years</t>
+  </si>
+  <si>
+    <t>70 years and older</t>
   </si>
 </sst>
 </file>
@@ -680,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F7C037-C9E8-4565-8747-61942B8DB76A}">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1764,6 +1797,18 @@
       <c r="I44" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="J44">
+        <v>8657</v>
+      </c>
+      <c r="K44">
+        <v>63.56</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H45" s="2">
@@ -1772,10 +1817,16 @@
       <c r="I45" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J45">
+        <v>4963</v>
+      </c>
+      <c r="K45">
+        <v>36.44</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
         <v>37</v>
@@ -1821,7 +1872,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B48" t="s">
         <v>39</v>
@@ -1867,7 +1918,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B50" t="s">
         <v>41</v>
@@ -1896,7 +1947,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B51" t="s">
         <v>43</v>
@@ -1925,7 +1976,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B52" t="s">
         <v>44</v>
@@ -1954,7 +2005,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B53" t="s">
         <v>45</v>
@@ -1983,7 +2034,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
         <v>46</v>
@@ -2053,6 +2104,160 @@
       </c>
       <c r="K57">
         <v>32.72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>36</v>
+      </c>
+      <c r="B58" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" t="s">
+        <v>95</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>54</v>
+      </c>
+      <c r="J58">
+        <v>13067</v>
+      </c>
+      <c r="K58">
+        <v>95.94</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H59" s="2">
+        <v>1</v>
+      </c>
+      <c r="I59" t="s">
+        <v>55</v>
+      </c>
+      <c r="J59">
+        <v>553</v>
+      </c>
+      <c r="K59">
+        <v>4.0599999999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>37</v>
+      </c>
+      <c r="B60" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" t="s">
+        <v>97</v>
+      </c>
+      <c r="D60" t="s">
+        <v>95</v>
+      </c>
+      <c r="H60" s="2">
+        <v>1</v>
+      </c>
+      <c r="I60" t="s">
+        <v>98</v>
+      </c>
+      <c r="J60">
+        <v>1054</v>
+      </c>
+      <c r="K60" s="3">
+        <f>J60/13620*100</f>
+        <v>7.7386196769456683</v>
+      </c>
+      <c r="L60">
+        <v>33</v>
+      </c>
+      <c r="M60" s="3">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H61" s="2">
+        <v>2</v>
+      </c>
+      <c r="I61" t="s">
+        <v>99</v>
+      </c>
+      <c r="J61">
+        <v>3179</v>
+      </c>
+      <c r="K61" s="3">
+        <f t="shared" ref="K61:K65" si="0">J61/13620*100</f>
+        <v>23.340675477239355</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H62" s="2">
+        <v>3</v>
+      </c>
+      <c r="I62" t="s">
+        <v>100</v>
+      </c>
+      <c r="J62">
+        <v>3136</v>
+      </c>
+      <c r="K62" s="3">
+        <f t="shared" si="0"/>
+        <v>23.024963289280471</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H63" s="2">
+        <v>4</v>
+      </c>
+      <c r="I63" t="s">
+        <v>101</v>
+      </c>
+      <c r="J63">
+        <v>3574</v>
+      </c>
+      <c r="K63" s="3">
+        <f t="shared" si="0"/>
+        <v>26.240822320117474</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H64" s="2">
+        <v>5</v>
+      </c>
+      <c r="I64" t="s">
+        <v>102</v>
+      </c>
+      <c r="J64">
+        <v>1936</v>
+      </c>
+      <c r="K64" s="3">
+        <f t="shared" si="0"/>
+        <v>14.214390602055801</v>
+      </c>
+    </row>
+    <row r="65" spans="8:11" x14ac:dyDescent="0.35">
+      <c r="H65" s="2">
+        <v>6</v>
+      </c>
+      <c r="I65" t="s">
+        <v>103</v>
+      </c>
+      <c r="J65">
+        <v>708</v>
+      </c>
+      <c r="K65" s="3">
+        <f t="shared" si="0"/>
+        <v>5.1982378854625555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>